<commit_message>
Update Activity Relationship table.xlsx
</commit_message>
<xml_diff>
--- a/documentation/Activity Relationship table.xlsx
+++ b/documentation/Activity Relationship table.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://tud365-my.sharepoint.com/personal/serenst_tudelft_nl/Documents/spatial computing architecture/CDS-Project/documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="389" documentId="8_{2C3C803F-6009-4E79-96C0-82548CC543AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{32678279-47F1-40B7-AA26-FB88290DB600}"/>
+  <xr:revisionPtr revIDLastSave="399" documentId="8_{2C3C803F-6009-4E79-96C0-82548CC543AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A8662C54-0189-431A-BBC4-8D1B751D5F98}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{69C57B10-3CF6-41E4-B6AD-BBD6308DA5D7}"/>
   </bookViews>
@@ -71,9 +71,6 @@
     <t>gym</t>
   </si>
   <si>
-    <t>Outside</t>
-  </si>
-  <si>
     <t>Gym</t>
   </si>
   <si>
@@ -96,6 +93,9 @@
   </si>
   <si>
     <t>wfef</t>
+  </si>
+  <si>
+    <t>Atrium</t>
   </si>
 </sst>
 </file>
@@ -151,6 +151,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -453,7 +457,7 @@
   <dimension ref="A1:O41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+      <selection activeCell="J22" sqref="J22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -482,7 +486,7 @@
         <v>6</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="I1" s="1" t="s">
         <v>7</v>
@@ -491,19 +495,19 @@
         <v>8</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="M1" s="1" t="s">
         <v>10</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>11</v>
+        <v>19</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.3">
@@ -511,7 +515,7 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C2">
         <v>5</v>
@@ -561,7 +565,7 @@
         <v>5</v>
       </c>
       <c r="C3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D3">
         <v>3</v>
@@ -594,7 +598,7 @@
         <v>2</v>
       </c>
       <c r="N3">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="O3">
         <v>2</v>
@@ -611,7 +615,7 @@
         <v>3</v>
       </c>
       <c r="D4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E4">
         <v>3</v>
@@ -641,7 +645,7 @@
         <v>2</v>
       </c>
       <c r="N4">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="O4">
         <v>1</v>
@@ -661,7 +665,7 @@
         <v>3</v>
       </c>
       <c r="E5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F5">
         <v>4</v>
@@ -711,7 +715,7 @@
         <v>4</v>
       </c>
       <c r="F6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G6">
         <v>4</v>
@@ -735,7 +739,7 @@
         <v>2</v>
       </c>
       <c r="N6">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="O6">
         <v>2</v>
@@ -761,7 +765,7 @@
         <v>4</v>
       </c>
       <c r="G7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H7">
         <v>2</v>
@@ -782,7 +786,7 @@
         <v>2</v>
       </c>
       <c r="N7">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="O7">
         <v>2</v>
@@ -811,7 +815,7 @@
         <v>2</v>
       </c>
       <c r="H8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I8">
         <v>2</v>
@@ -861,7 +865,7 @@
         <v>2</v>
       </c>
       <c r="I9" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="J9">
         <v>4</v>
@@ -911,7 +915,7 @@
         <v>4</v>
       </c>
       <c r="J10" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="K10">
         <v>2</v>
@@ -931,7 +935,7 @@
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B11">
         <v>1</v>
@@ -961,7 +965,7 @@
         <v>2</v>
       </c>
       <c r="K11" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="L11">
         <v>3</v>
@@ -1011,7 +1015,7 @@
         <v>3</v>
       </c>
       <c r="L12" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="M12">
         <v>2</v>
@@ -1025,7 +1029,7 @@
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B13">
         <v>2</v>
@@ -1061,7 +1065,7 @@
         <v>2</v>
       </c>
       <c r="M13" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="N13">
         <v>3</v>
@@ -1072,25 +1076,25 @@
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>11</v>
+        <v>19</v>
       </c>
       <c r="B14">
         <v>2</v>
       </c>
       <c r="C14">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D14">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E14">
         <v>2</v>
       </c>
       <c r="F14">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="G14">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="H14">
         <v>2</v>
@@ -1111,7 +1115,7 @@
         <v>3</v>
       </c>
       <c r="N14" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="O14">
         <v>2</v>
@@ -1119,7 +1123,7 @@
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B15">
         <v>1</v>
@@ -1161,19 +1165,19 @@
         <v>2</v>
       </c>
       <c r="O15" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="21" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B21" t="str">
-        <f t="shared" ref="B20:B33" si="0">CONCATENATE(B3,",",C3,",",D3,",",E3,",",F3,",",G3,",",H3,",",I3,",",J3,",",K3,",",L3,",",M3,",",N3,",",O3)</f>
-        <v>5,Self,3,4,3,3,3,2,1,2,1,2,3,2</v>
+        <f t="shared" ref="B21:B33" si="0">CONCATENATE(B3,",",C3,",",D3,",",E3,",",F3,",",G3,",",H3,",",I3,",",J3,",",K3,",",L3,",",M3,",",N3,",",O3)</f>
+        <v>5,Self,3,4,3,3,3,2,1,2,1,2,4,2</v>
       </c>
     </row>
     <row r="22" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B22" t="str">
         <f t="shared" si="0"/>
-        <v>5,3,Self,3,2,2,4,2,1,3,1,2,2,1</v>
+        <v>5,3,Self,3,2,2,4,2,1,3,1,2,4,1</v>
       </c>
     </row>
     <row r="23" spans="2:2" x14ac:dyDescent="0.3">
@@ -1185,13 +1189,13 @@
     <row r="24" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B24" t="str">
         <f t="shared" si="0"/>
-        <v>5,3,2,4,Self,4,2,4,3,2,1,2,3,2</v>
+        <v>5,3,2,4,Self,4,2,4,3,2,1,2,4,2</v>
       </c>
     </row>
     <row r="25" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B25" t="str">
         <f t="shared" si="0"/>
-        <v>5,3,2,3,4,Self,2,4,4,2,1,2,3,2</v>
+        <v>5,3,2,3,4,Self,2,4,4,2,1,2,4,2</v>
       </c>
     </row>
     <row r="26" spans="2:2" x14ac:dyDescent="0.3">
@@ -1233,7 +1237,7 @@
     <row r="32" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B32" t="str">
         <f t="shared" si="0"/>
-        <v>2,3,2,2,3,3,2,2,4,3,3,3,Self,2</v>
+        <v>2,4,4,2,4,4,2,2,4,3,3,3,Self,2</v>
       </c>
     </row>
     <row r="33" spans="2:4" x14ac:dyDescent="0.3">
@@ -1244,7 +1248,7 @@
     </row>
     <row r="41" spans="2:4" x14ac:dyDescent="0.3">
       <c r="D41" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
entree verandered naar entrance
</commit_message>
<xml_diff>
--- a/documentation/Activity Relationship table.xlsx
+++ b/documentation/Activity Relationship table.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://tud365-my.sharepoint.com/personal/serenst_tudelft_nl/Documents/spatial computing architecture/CDS-Project/documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="399" documentId="8_{2C3C803F-6009-4E79-96C0-82548CC543AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A8662C54-0189-431A-BBC4-8D1B751D5F98}"/>
+  <xr:revisionPtr revIDLastSave="401" documentId="8_{2C3C803F-6009-4E79-96C0-82548CC543AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1D2915D7-2F67-48D2-8145-84D9C81A132F}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{69C57B10-3CF6-41E4-B6AD-BBD6308DA5D7}"/>
   </bookViews>
@@ -38,9 +38,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="20">
   <si>
-    <t>Housing entree</t>
-  </si>
-  <si>
     <t>Starter houses</t>
   </si>
   <si>
@@ -96,6 +93,9 @@
   </si>
   <si>
     <t>Atrium</t>
+  </si>
+  <si>
+    <t>Housing entrance</t>
   </si>
 </sst>
 </file>
@@ -457,7 +457,7 @@
   <dimension ref="A1:O41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J22" sqref="J22"/>
+      <selection activeCell="M20" sqref="M20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -468,54 +468,54 @@
   <sheetData>
     <row r="1" spans="1:15" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>1</v>
-      </c>
       <c r="D1" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="J1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="L1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="I1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="K1" s="1" t="s">
+      <c r="M1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="O1" s="1" t="s">
         <v>12</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>0</v>
+        <v>19</v>
       </c>
       <c r="B2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C2">
         <v>5</v>
@@ -559,13 +559,13 @@
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B3">
         <v>5</v>
       </c>
       <c r="C3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D3">
         <v>3</v>
@@ -606,7 +606,7 @@
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B4">
         <v>5</v>
@@ -615,7 +615,7 @@
         <v>3</v>
       </c>
       <c r="D4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E4">
         <v>3</v>
@@ -653,7 +653,7 @@
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B5">
         <v>4</v>
@@ -665,7 +665,7 @@
         <v>3</v>
       </c>
       <c r="E5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F5">
         <v>4</v>
@@ -700,7 +700,7 @@
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B6">
         <v>5</v>
@@ -715,7 +715,7 @@
         <v>4</v>
       </c>
       <c r="F6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G6">
         <v>4</v>
@@ -747,7 +747,7 @@
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B7">
         <v>5</v>
@@ -765,7 +765,7 @@
         <v>4</v>
       </c>
       <c r="G7" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H7">
         <v>2</v>
@@ -794,7 +794,7 @@
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B8">
         <v>3</v>
@@ -815,7 +815,7 @@
         <v>2</v>
       </c>
       <c r="H8" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="I8">
         <v>2</v>
@@ -841,7 +841,7 @@
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B9">
         <v>2</v>
@@ -865,7 +865,7 @@
         <v>2</v>
       </c>
       <c r="I9" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="J9">
         <v>4</v>
@@ -888,7 +888,7 @@
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B10">
         <v>3</v>
@@ -915,7 +915,7 @@
         <v>4</v>
       </c>
       <c r="J10" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="K10">
         <v>2</v>
@@ -935,7 +935,7 @@
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B11">
         <v>1</v>
@@ -965,7 +965,7 @@
         <v>2</v>
       </c>
       <c r="K11" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="L11">
         <v>3</v>
@@ -982,7 +982,7 @@
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B12">
         <v>1</v>
@@ -1015,7 +1015,7 @@
         <v>3</v>
       </c>
       <c r="L12" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="M12">
         <v>2</v>
@@ -1029,7 +1029,7 @@
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B13">
         <v>2</v>
@@ -1065,7 +1065,7 @@
         <v>2</v>
       </c>
       <c r="M13" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="N13">
         <v>3</v>
@@ -1076,7 +1076,7 @@
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B14">
         <v>2</v>
@@ -1115,7 +1115,7 @@
         <v>3</v>
       </c>
       <c r="N14" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="O14">
         <v>2</v>
@@ -1123,7 +1123,7 @@
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B15">
         <v>1</v>
@@ -1165,7 +1165,7 @@
         <v>2</v>
       </c>
       <c r="O15" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="21" spans="2:2" x14ac:dyDescent="0.3">
@@ -1248,7 +1248,7 @@
     </row>
     <row r="41" spans="2:4" x14ac:dyDescent="0.3">
       <c r="D41" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
CSV files made and imported
</commit_message>
<xml_diff>
--- a/documentation/Activity Relationship table.xlsx
+++ b/documentation/Activity Relationship table.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://tud365-my.sharepoint.com/personal/serenst_tudelft_nl/Documents/spatial computing architecture/CDS-Project/documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="401" documentId="8_{2C3C803F-6009-4E79-96C0-82548CC543AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1D2915D7-2F67-48D2-8145-84D9C81A132F}"/>
+  <xr:revisionPtr revIDLastSave="402" documentId="8_{2C3C803F-6009-4E79-96C0-82548CC543AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{29F9D8C4-A709-4C06-8944-E60365C9E00D}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{69C57B10-3CF6-41E4-B6AD-BBD6308DA5D7}"/>
   </bookViews>
@@ -456,8 +456,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D40333D7-3B21-4950-BD3A-61315E73F84F}">
   <dimension ref="A1:O41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M20" sqref="M20"/>
+    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="B21" sqref="B21:C33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1170,13 +1170,13 @@
     </row>
     <row r="21" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B21" t="str">
-        <f t="shared" ref="B21:B33" si="0">CONCATENATE(B3,",",C3,",",D3,",",E3,",",F3,",",G3,",",H3,",",I3,",",J3,",",K3,",",L3,",",M3,",",N3,",",O3)</f>
+        <f>CONCATENATE(B3,",",C3,",",D3,",",E3,",",F3,",",G3,",",H3,",",I3,",",J3,",",K3,",",L3,",",M3,",",N3,",",O3)</f>
         <v>5,Self,3,4,3,3,3,2,1,2,1,2,4,2</v>
       </c>
     </row>
     <row r="22" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B22" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="B21:B33" si="0">CONCATENATE(B4,",",C4,",",D4,",",E4,",",F4,",",G4,",",H4,",",I4,",",J4,",",K4,",",L4,",",M4,",",N4,",",O4)</f>
         <v>5,3,Self,3,2,2,4,2,1,3,1,2,4,1</v>
       </c>
     </row>

</xml_diff>